<commit_message>
fix 1cut level function,
</commit_message>
<xml_diff>
--- a/Others/TestCuts/TestCut2MIP/pre_cut2_analysis.xlsx
+++ b/Others/TestCuts/TestCut2MIP/pre_cut2_analysis.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="119">
   <si>
     <t>Sc(N/M)</t>
   </si>
@@ -374,6 +374,9 @@
   </si>
   <si>
     <t>TimeDev%</t>
+  </si>
+  <si>
+    <t>Cut2_Moretime</t>
   </si>
 </sst>
 </file>
@@ -990,59 +993,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="184731" cy="264560"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14497050" y="180975"/>
-          <a:ext cx="184731" cy="264560"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr lang="fr-FR" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4376677" cy="436786"/>
     <xdr:sp macro="" textlink="">
@@ -1052,7 +1006,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14135100" y="76200"/>
+          <a:off x="13515975" y="295275"/>
           <a:ext cx="4376677" cy="436786"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1363,8 +1317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S134"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="Q121" sqref="Q121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1424,7 +1378,9 @@
       <c r="O1" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="Q1" s="18"/>
+      <c r="Q1" s="18" t="s">
+        <v>118</v>
+      </c>
       <c r="R1" s="18"/>
       <c r="S1" s="18"/>
     </row>
@@ -1480,7 +1436,10 @@
         <f>IF( OR(M3=0, N3=""), "", (N3-M3)/M3*100)</f>
         <v/>
       </c>
-      <c r="Q3" s="18"/>
+      <c r="Q3" s="18" t="str">
+        <f>IF( AND(I3&gt;J3, N3&lt;M3), "ici", "")</f>
+        <v/>
+      </c>
       <c r="R3" s="18"/>
       <c r="S3" s="18"/>
     </row>
@@ -1527,7 +1486,10 @@
         <f t="shared" ref="O4:O67" si="2">IF( OR(M4=0, N4=""), "", (N4-M4)/M4*100)</f>
         <v/>
       </c>
-      <c r="Q4" s="18"/>
+      <c r="Q4" s="18" t="str">
+        <f t="shared" ref="Q4:Q67" si="3">IF( AND(I4&gt;J4, N4&lt;M4), "ici", "")</f>
+        <v/>
+      </c>
       <c r="R4" s="18"/>
       <c r="S4" s="18"/>
     </row>
@@ -1574,7 +1536,10 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="Q5" s="18"/>
+      <c r="Q5" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="R5" s="18"/>
       <c r="S5" s="18"/>
     </row>
@@ -1621,6 +1586,10 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="Q6" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -1665,6 +1634,10 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="Q7" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1709,6 +1682,10 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="Q8" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
@@ -1753,6 +1730,10 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="Q9" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
@@ -1797,6 +1778,10 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="Q10" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
@@ -1841,6 +1826,10 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="Q11" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
@@ -1885,6 +1874,10 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="Q12" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
@@ -1929,6 +1922,10 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="Q13" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>ici</v>
+      </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
@@ -1973,6 +1970,10 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="Q14" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
@@ -2017,6 +2018,10 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
+      <c r="Q15" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
@@ -2061,8 +2066,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q16" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>34</v>
       </c>
@@ -2105,8 +2114,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q17" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>ici</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I18" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2119,8 +2132,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q18" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>35</v>
       </c>
@@ -2163,8 +2180,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q19" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>36</v>
       </c>
@@ -2207,8 +2228,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q20" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>102</v>
       </c>
@@ -2251,8 +2276,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q21" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I22" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2265,8 +2294,12 @@
         <f>IF( OR(M22=0, N22=""), "", (N22-M22)/M22*100)</f>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q22" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I23" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2279,8 +2312,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q23" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I24" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2293,8 +2330,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q24" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I25" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2307,8 +2348,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q25" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I26" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2321,8 +2366,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q26" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>37</v>
       </c>
@@ -2365,8 +2414,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q27" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>38</v>
       </c>
@@ -2409,8 +2462,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q28" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I29" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2426,8 +2483,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q29" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>39</v>
       </c>
@@ -2470,8 +2531,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q30" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I31" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2487,8 +2552,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q31" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>40</v>
       </c>
@@ -2531,8 +2600,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q32" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>41</v>
       </c>
@@ -2575,8 +2648,12 @@
         <f t="shared" si="2"/>
         <v>12.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q33" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>42</v>
       </c>
@@ -2619,8 +2696,12 @@
         <f>IF( OR(M34=0, N34=""), "", (N34-M34)/M34*100)</f>
         <v/>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q34" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>43</v>
       </c>
@@ -2663,8 +2744,12 @@
         <f t="shared" si="2"/>
         <v>-3.225806451612903</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q35" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v>ici</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>44</v>
       </c>
@@ -2707,8 +2792,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q36" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I37" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2721,8 +2810,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q37" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>45</v>
       </c>
@@ -2765,8 +2858,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q38" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>46</v>
       </c>
@@ -2809,8 +2906,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q39" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>47</v>
       </c>
@@ -2853,8 +2954,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q40" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I41" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2867,8 +2972,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q41" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>48</v>
       </c>
@@ -2911,8 +3020,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q42" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>49</v>
       </c>
@@ -2955,8 +3068,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q43" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I44" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2969,8 +3086,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q44" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>50</v>
       </c>
@@ -3013,8 +3134,12 @@
         <f t="shared" si="2"/>
         <v>-100</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q45" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
         <v>51</v>
       </c>
@@ -3057,8 +3182,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q46" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>52</v>
       </c>
@@ -3101,8 +3230,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q47" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>53</v>
       </c>
@@ -3145,8 +3278,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q48" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
         <v>54</v>
       </c>
@@ -3189,8 +3326,12 @@
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q49" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>55</v>
       </c>
@@ -3233,8 +3374,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q50" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>56</v>
       </c>
@@ -3277,8 +3422,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q51" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
         <v>57</v>
       </c>
@@ -3321,8 +3470,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q52" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
         <v>58</v>
       </c>
@@ -3365,8 +3518,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q53" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>59</v>
       </c>
@@ -3409,8 +3566,12 @@
         <f t="shared" si="2"/>
         <v>24.637681159420293</v>
       </c>
-    </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q54" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
         <v>60</v>
       </c>
@@ -3453,8 +3614,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q55" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
         <v>61</v>
       </c>
@@ -3497,8 +3662,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q56" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>62</v>
       </c>
@@ -3541,8 +3710,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q57" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
         <v>63</v>
       </c>
@@ -3585,8 +3758,12 @@
         <f t="shared" si="2"/>
         <v>-22.394200626959247</v>
       </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q58" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
         <v>64</v>
       </c>
@@ -3629,8 +3806,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q59" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>65</v>
       </c>
@@ -3673,8 +3854,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q60" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
         <v>103</v>
       </c>
@@ -3717,8 +3902,12 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q61" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
         <v>66</v>
       </c>
@@ -3761,8 +3950,12 @@
         <f t="shared" si="2"/>
         <v>59.976976208749043</v>
       </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q62" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>67</v>
       </c>
@@ -3805,8 +3998,12 @@
         <f t="shared" si="2"/>
         <v>-31.217273854237977</v>
       </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q63" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
         <v>68</v>
       </c>
@@ -3849,8 +4046,12 @@
         <f t="shared" si="2"/>
         <v>-20.72655589974655</v>
       </c>
-    </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q64" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
         <v>69</v>
       </c>
@@ -3893,8 +4094,12 @@
         <f t="shared" si="2"/>
         <v>95.302013422818789</v>
       </c>
-    </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q65" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="4" t="s">
         <v>70</v>
       </c>
@@ -3937,8 +4142,12 @@
         <f t="shared" si="2"/>
         <v>-26.950354609929079</v>
       </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q66" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
         <v>71</v>
       </c>
@@ -3981,8 +4190,12 @@
         <f t="shared" si="2"/>
         <v>6.3396952211865658</v>
       </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q67" s="18" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="4" t="s">
         <v>72</v>
       </c>
@@ -4005,14 +4218,14 @@
         <v>1.51</v>
       </c>
       <c r="I68" s="8">
-        <f t="shared" ref="I68:I121" si="3">IF(G68="", "", G68-H68)</f>
+        <f t="shared" ref="I68:I121" si="4">IF(G68="", "", G68-H68)</f>
         <v>5.13</v>
       </c>
       <c r="J68" s="8">
         <v>3.98</v>
       </c>
       <c r="K68" s="9">
-        <f t="shared" ref="K68:K121" si="4">IF(J68="", "", (I68-J68)/J68*100)</f>
+        <f t="shared" ref="K68:K121" si="5">IF(J68="", "", (I68-J68)/J68*100)</f>
         <v>28.894472361809044</v>
       </c>
       <c r="M68" s="14">
@@ -4022,11 +4235,15 @@
         <v>41</v>
       </c>
       <c r="O68" s="17">
-        <f t="shared" ref="O68:O121" si="5">IF( OR(M68=0, N68=""), "", (N68-M68)/M68*100)</f>
+        <f t="shared" ref="O68:O121" si="6">IF( OR(M68=0, N68=""), "", (N68-M68)/M68*100)</f>
         <v>-71.328671328671334</v>
       </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q68" s="18" t="str">
+        <f t="shared" ref="Q68:Q121" si="7">IF( AND(I68&gt;J68, N68&lt;M68), "ici", "")</f>
+        <v>ici</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>73</v>
       </c>
@@ -4049,14 +4266,14 @@
         <v>1.48</v>
       </c>
       <c r="I69" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.5399999999999996</v>
       </c>
       <c r="J69" s="8">
         <v>2.56</v>
       </c>
       <c r="K69" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.78125000000001799</v>
       </c>
       <c r="M69" s="14">
@@ -4066,11 +4283,15 @@
         <v>0</v>
       </c>
       <c r="O69" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q69" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
         <v>74</v>
       </c>
@@ -4093,14 +4314,14 @@
         <v>0.91</v>
       </c>
       <c r="I70" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.48999999999999988</v>
       </c>
       <c r="J70" s="8">
         <v>1.1200000000000001</v>
       </c>
       <c r="K70" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-56.250000000000014</v>
       </c>
       <c r="M70" s="14">
@@ -4110,11 +4331,15 @@
         <v>0</v>
       </c>
       <c r="O70" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q70" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
         <v>75</v>
       </c>
@@ -4137,14 +4362,14 @@
         <v>2.3199999999999998</v>
       </c>
       <c r="I71" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>109.72000000000001</v>
       </c>
       <c r="J71" s="8">
         <v>65.47</v>
       </c>
       <c r="K71" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>67.588208339697601</v>
       </c>
       <c r="M71" s="14">
@@ -4154,11 +4379,15 @@
         <v>4164</v>
       </c>
       <c r="O71" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-28.318127044241692</v>
       </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q71" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>ici</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
         <v>76</v>
       </c>
@@ -4181,14 +4410,14 @@
         <v>1.94</v>
       </c>
       <c r="I72" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>11.32</v>
       </c>
       <c r="J72" s="8">
         <v>11.65</v>
       </c>
       <c r="K72" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-2.8326180257510734</v>
       </c>
       <c r="M72" s="14">
@@ -4198,11 +4427,15 @@
         <v>874</v>
       </c>
       <c r="O72" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-22.311111111111114</v>
       </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q72" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
         <v>77</v>
       </c>
@@ -4225,14 +4458,14 @@
         <v>2.73</v>
       </c>
       <c r="I73" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.329999999999998</v>
       </c>
       <c r="J73" s="8">
         <v>20.58</v>
       </c>
       <c r="K73" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-25.510204081632654</v>
       </c>
       <c r="M73" s="14">
@@ -4242,11 +4475,15 @@
         <v>1334</v>
       </c>
       <c r="O73" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-57.07850707850708</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q73" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
         <v>78</v>
       </c>
@@ -4269,14 +4506,14 @@
         <v>3.15</v>
       </c>
       <c r="I74" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>25.540000000000003</v>
       </c>
       <c r="J74" s="8">
         <v>71.040000000000006</v>
       </c>
       <c r="K74" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-64.048423423423415</v>
       </c>
       <c r="M74" s="14">
@@ -4286,11 +4523,15 @@
         <v>2179</v>
       </c>
       <c r="O74" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-45.782532968400098</v>
       </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q74" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>79</v>
       </c>
@@ -4313,14 +4554,14 @@
         <v>1.76</v>
       </c>
       <c r="I75" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10.86</v>
       </c>
       <c r="J75" s="8">
         <v>10.050000000000001</v>
       </c>
       <c r="K75" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.0597014925373003</v>
       </c>
       <c r="M75" s="14">
@@ -4330,11 +4571,15 @@
         <v>235</v>
       </c>
       <c r="O75" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-47.544642857142854</v>
       </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q75" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>ici</v>
+      </c>
+    </row>
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>80</v>
       </c>
@@ -4357,25 +4602,29 @@
         <v>2.34</v>
       </c>
       <c r="I76" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.01</v>
       </c>
       <c r="J76" s="8">
         <v>4.95</v>
       </c>
       <c r="K76" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.2121212121212042</v>
       </c>
       <c r="N76" s="15">
         <v>56</v>
       </c>
       <c r="O76" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q76" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>81</v>
       </c>
@@ -4398,14 +4647,14 @@
         <v>1.83</v>
       </c>
       <c r="I77" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>15.610000000000001</v>
       </c>
       <c r="J77" s="8">
         <v>16.329999999999998</v>
       </c>
       <c r="K77" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-4.4090630740967374</v>
       </c>
       <c r="M77" s="14">
@@ -4415,11 +4664,15 @@
         <v>604</v>
       </c>
       <c r="O77" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-26.251526251526254</v>
       </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q77" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
         <v>82</v>
       </c>
@@ -4442,14 +4695,14 @@
         <v>3.78</v>
       </c>
       <c r="I78" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>132.03</v>
       </c>
       <c r="J78" s="8">
         <v>117.55</v>
       </c>
       <c r="K78" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>12.318162484049344</v>
       </c>
       <c r="M78" s="14">
@@ -4459,11 +4712,15 @@
         <v>4107</v>
       </c>
       <c r="O78" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>27.309361438313701</v>
       </c>
-    </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q78" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
         <v>83</v>
       </c>
@@ -4486,14 +4743,14 @@
         <v>1.08</v>
       </c>
       <c r="I79" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>13.33</v>
       </c>
       <c r="J79" s="8">
         <v>8.8000000000000007</v>
       </c>
       <c r="K79" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>51.47727272727272</v>
       </c>
       <c r="M79" s="14">
@@ -4503,11 +4760,15 @@
         <v>992</v>
       </c>
       <c r="O79" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-42.459396751740144</v>
       </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q79" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>ici</v>
+      </c>
+    </row>
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
         <v>84</v>
       </c>
@@ -4530,14 +4791,14 @@
         <v>1.78</v>
       </c>
       <c r="I80" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>8.7800000000000011</v>
       </c>
       <c r="J80" s="8">
         <v>9.9499999999999993</v>
       </c>
       <c r="K80" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-11.758793969849227</v>
       </c>
       <c r="M80" s="14">
@@ -4547,11 +4808,15 @@
         <v>274</v>
       </c>
       <c r="O80" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-46.37964774951076</v>
       </c>
-    </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q80" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
         <v>104</v>
       </c>
@@ -4574,14 +4839,14 @@
         <v>2.59</v>
       </c>
       <c r="I81" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.9399999999999995</v>
       </c>
       <c r="J81" s="8">
         <v>4.43</v>
       </c>
       <c r="K81" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>34.085778781038371</v>
       </c>
       <c r="M81" s="14">
@@ -4591,53 +4856,69 @@
         <v>417</v>
       </c>
       <c r="O81" s="17">
+        <f t="shared" si="6"/>
+        <v>48.928571428571423</v>
+      </c>
+      <c r="Q81" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I82" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K82" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>48.928571428571423</v>
-      </c>
-    </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I82" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K82" s="9" t="str">
+        <v/>
+      </c>
+      <c r="O82" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q82" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I83" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="O82" s="17" t="str">
+      <c r="K83" s="9" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I83" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K83" s="9" t="str">
+      <c r="O83" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q83" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I84" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="O83" s="17" t="str">
+      <c r="K84" s="9" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I84" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K84" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="O84" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q84" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
         <v>85</v>
       </c>
@@ -4660,14 +4941,14 @@
         <v>0.98</v>
       </c>
       <c r="I85" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>98.31</v>
       </c>
       <c r="J85" s="8">
         <v>110.95</v>
       </c>
       <c r="K85" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-11.392519152771518</v>
       </c>
       <c r="M85" s="14">
@@ -4677,11 +4958,15 @@
         <v>2897</v>
       </c>
       <c r="O85" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-28.18542389687655</v>
       </c>
-    </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q85" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
         <v>86</v>
       </c>
@@ -4704,14 +4989,14 @@
         <v>0.95</v>
       </c>
       <c r="I86" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>58.919999999999995</v>
       </c>
       <c r="J86" s="8">
         <v>23.1</v>
       </c>
       <c r="K86" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>155.06493506493501</v>
       </c>
       <c r="M86" s="14">
@@ -4721,39 +5006,51 @@
         <v>7174</v>
       </c>
       <c r="O86" s="17">
+        <f t="shared" si="6"/>
+        <v>52.217271377042216</v>
+      </c>
+      <c r="Q86" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I87" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K87" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>52.217271377042216</v>
-      </c>
-    </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I87" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K87" s="9" t="str">
+        <v/>
+      </c>
+      <c r="O87" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q87" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I88" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="O87" s="17" t="str">
+      <c r="K88" s="9" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I88" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K88" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="O88" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q88" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
         <v>87</v>
       </c>
@@ -4776,14 +5073,14 @@
         <v>6.65</v>
       </c>
       <c r="I89" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>529.4</v>
       </c>
       <c r="J89" s="8">
         <v>415.19</v>
       </c>
       <c r="K89" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>27.507887954912203</v>
       </c>
       <c r="M89" s="14">
@@ -4793,25 +5090,33 @@
         <v>14680</v>
       </c>
       <c r="O89" s="17">
+        <f t="shared" si="6"/>
+        <v>60.297008080366886</v>
+      </c>
+      <c r="Q89" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I90" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K90" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>60.297008080366886</v>
-      </c>
-    </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I90" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K90" s="9" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O90" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q90" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
         <v>88</v>
       </c>
@@ -4834,14 +5139,14 @@
         <v>3.82</v>
       </c>
       <c r="I91" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>641.9799999999999</v>
       </c>
       <c r="J91" s="8">
         <v>757.19</v>
       </c>
       <c r="K91" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-15.215467716161088</v>
       </c>
       <c r="M91" s="14">
@@ -4851,11 +5156,15 @@
         <v>26336</v>
       </c>
       <c r="O91" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-60.806607634496615</v>
       </c>
-    </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q91" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
         <v>89</v>
       </c>
@@ -4878,14 +5187,14 @@
         <v>3.59</v>
       </c>
       <c r="I92" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1800.4</v>
       </c>
       <c r="J92" s="8">
         <v>1765.22</v>
       </c>
       <c r="K92" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.9929527197743091</v>
       </c>
       <c r="M92" s="14">
@@ -4895,11 +5204,15 @@
         <v>33313</v>
       </c>
       <c r="O92" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-48.864089890400024</v>
       </c>
-    </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q92" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>ici</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
         <v>90</v>
       </c>
@@ -4922,14 +5235,14 @@
         <v>1.84</v>
       </c>
       <c r="I93" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>785.6</v>
       </c>
       <c r="J93" s="8">
         <v>769.13</v>
       </c>
       <c r="K93" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.1413805208482346</v>
       </c>
       <c r="M93" s="14">
@@ -4939,11 +5252,15 @@
         <v>25638</v>
       </c>
       <c r="O93" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-7.9888027562446169</v>
       </c>
-    </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q93" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>ici</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
         <v>91</v>
       </c>
@@ -4966,14 +5283,14 @@
         <v>1.92</v>
       </c>
       <c r="I94" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>94.46</v>
       </c>
       <c r="J94" s="8">
         <v>68.13</v>
       </c>
       <c r="K94" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>38.646704829003376</v>
       </c>
       <c r="M94" s="14">
@@ -4983,11 +5300,15 @@
         <v>1831</v>
       </c>
       <c r="O94" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-46.226138032305428</v>
       </c>
-    </row>
-    <row r="95" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q94" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>ici</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
         <v>92</v>
       </c>
@@ -5010,14 +5331,14 @@
         <v>2.9</v>
       </c>
       <c r="I95" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1800.35</v>
       </c>
       <c r="J95" s="8">
         <v>1516.04</v>
       </c>
       <c r="K95" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>18.753462969314789</v>
       </c>
       <c r="M95" s="14">
@@ -5027,25 +5348,33 @@
         <v>17680</v>
       </c>
       <c r="O95" s="17">
+        <f t="shared" si="6"/>
+        <v>-11.600000000000001</v>
+      </c>
+      <c r="Q95" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>ici</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I96" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K96" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>-11.600000000000001</v>
-      </c>
-    </row>
-    <row r="96" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I96" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K96" s="9" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O96" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q96" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>93</v>
       </c>
@@ -5068,14 +5397,14 @@
         <v>2.42</v>
       </c>
       <c r="I97" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>263.75</v>
       </c>
       <c r="J97" s="8">
         <v>245.98</v>
       </c>
       <c r="K97" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.2241645662249017</v>
       </c>
       <c r="M97" s="14">
@@ -5085,25 +5414,33 @@
         <v>40001</v>
       </c>
       <c r="O97" s="17">
+        <f t="shared" si="6"/>
+        <v>9.0777705061082035</v>
+      </c>
+      <c r="Q97" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I98" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K98" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>9.0777705061082035</v>
-      </c>
-    </row>
-    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I98" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K98" s="9" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O98" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q98" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
         <v>94</v>
       </c>
@@ -5126,14 +5463,14 @@
         <v>2.09</v>
       </c>
       <c r="I99" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>265.64000000000004</v>
       </c>
       <c r="J99" s="8">
         <v>340.2</v>
       </c>
       <c r="K99" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-21.916519694297456</v>
       </c>
       <c r="M99" s="14">
@@ -5143,109 +5480,141 @@
         <v>3071</v>
       </c>
       <c r="O99" s="17">
+        <f t="shared" si="6"/>
+        <v>-41.925113464447804</v>
+      </c>
+      <c r="Q99" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I100" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K100" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>-41.925113464447804</v>
-      </c>
-    </row>
-    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I100" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K100" s="9" t="str">
+        <v/>
+      </c>
+      <c r="O100" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q100" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I101" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="O100" s="17" t="str">
+      <c r="K101" s="9" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I101" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K101" s="9" t="str">
+      <c r="O101" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q101" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I102" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="O101" s="17" t="str">
+      <c r="K102" s="9" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I102" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K102" s="9" t="str">
+      <c r="O102" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q102" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I103" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="O102" s="17" t="str">
+      <c r="K103" s="9" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I103" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K103" s="9" t="str">
+      <c r="O103" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q103" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I104" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="O103" s="17" t="str">
+      <c r="K104" s="9" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I104" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K104" s="9" t="str">
+      <c r="O104" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q104" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I105" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="O104" s="17" t="str">
+      <c r="K105" s="9" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I105" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K105" s="9" t="str">
+      <c r="O105" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q105" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I106" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="O105" s="17" t="str">
+      <c r="K106" s="9" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I106" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K106" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="O106" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q106" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A107" s="4" t="s">
         <v>95</v>
       </c>
@@ -5268,14 +5637,14 @@
         <v>5.69</v>
       </c>
       <c r="I107" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>167.05</v>
       </c>
       <c r="J107" s="8">
         <v>124.91</v>
       </c>
       <c r="K107" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>33.736290128892819</v>
       </c>
       <c r="M107" s="14">
@@ -5285,67 +5654,87 @@
         <v>6816</v>
       </c>
       <c r="O107" s="17">
+        <f t="shared" si="6"/>
+        <v>-27.171706378886633</v>
+      </c>
+      <c r="Q107" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>ici</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I108" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K108" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>-27.171706378886633</v>
-      </c>
-    </row>
-    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I108" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K108" s="9" t="str">
+        <v/>
+      </c>
+      <c r="O108" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q108" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I109" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="O108" s="17" t="str">
+      <c r="K109" s="9" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="109" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I109" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K109" s="9" t="str">
+      <c r="O109" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q109" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I110" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="O109" s="17" t="str">
+      <c r="K110" s="9" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I110" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K110" s="9" t="str">
+      <c r="O110" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q110" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I111" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="O110" s="17" t="str">
+      <c r="K111" s="9" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I111" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K111" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="O111" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q111" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="4" t="s">
         <v>96</v>
       </c>
@@ -5368,14 +5757,14 @@
         <v>5.24</v>
       </c>
       <c r="I112" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>353.05</v>
       </c>
       <c r="J112" s="8">
         <v>456.08</v>
       </c>
       <c r="K112" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-22.590335028942285</v>
       </c>
       <c r="M112" s="14">
@@ -5385,11 +5774,15 @@
         <v>10468</v>
       </c>
       <c r="O112" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-33.150265023309281</v>
       </c>
-    </row>
-    <row r="113" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q112" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="4" t="s">
         <v>97</v>
       </c>
@@ -5412,14 +5805,14 @@
         <v>5.13</v>
       </c>
       <c r="I113" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>156.77000000000001</v>
       </c>
       <c r="J113" s="8">
         <v>136.76</v>
       </c>
       <c r="K113" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>14.631471190406566</v>
       </c>
       <c r="M113" s="14">
@@ -5429,53 +5822,69 @@
         <v>8838</v>
       </c>
       <c r="O113" s="17">
+        <f t="shared" si="6"/>
+        <v>-33.573844419391207</v>
+      </c>
+      <c r="Q113" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>ici</v>
+      </c>
+    </row>
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I114" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K114" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>-33.573844419391207</v>
-      </c>
-    </row>
-    <row r="114" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I114" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K114" s="9" t="str">
+        <v/>
+      </c>
+      <c r="O114" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q114" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I115" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="O114" s="17" t="str">
+      <c r="K115" s="9" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="115" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I115" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K115" s="9" t="str">
+      <c r="O115" s="17" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q115" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I116" s="8" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="O115" s="17" t="str">
+      <c r="K116" s="9" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-    </row>
-    <row r="116" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I116" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K116" s="9" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
       <c r="O116" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="117" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q116" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" s="4" t="s">
         <v>98</v>
       </c>
@@ -5498,14 +5907,14 @@
         <v>9.08</v>
       </c>
       <c r="I117" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1313.0800000000002</v>
       </c>
       <c r="J117" s="8">
         <v>1788.43</v>
       </c>
       <c r="K117" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-26.579178385511309</v>
       </c>
       <c r="M117" s="14">
@@ -5515,25 +5924,33 @@
         <v>11930</v>
       </c>
       <c r="O117" s="17">
+        <f t="shared" si="6"/>
+        <v>-17.502247424106216</v>
+      </c>
+      <c r="Q117" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I118" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K118" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>-17.502247424106216</v>
-      </c>
-    </row>
-    <row r="118" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I118" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K118" s="9" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O118" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="119" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q118" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A119" s="4" t="s">
         <v>99</v>
       </c>
@@ -5556,14 +5973,14 @@
         <v>19.079999999999998</v>
       </c>
       <c r="I119" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>326.51</v>
       </c>
       <c r="J119" s="8">
         <v>193.47</v>
       </c>
       <c r="K119" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>68.765183232542498</v>
       </c>
       <c r="M119" s="14">
@@ -5573,25 +5990,33 @@
         <v>7272</v>
       </c>
       <c r="O119" s="17">
+        <f t="shared" si="6"/>
+        <v>48.711656441717793</v>
+      </c>
+      <c r="Q119" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="I120" s="8" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="K120" s="9" t="str">
         <f t="shared" si="5"/>
-        <v>48.711656441717793</v>
-      </c>
-    </row>
-    <row r="120" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I120" s="8" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="K120" s="9" t="str">
-        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="O120" s="17" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="121" spans="1:15" x14ac:dyDescent="0.25">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="Q120" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A121" s="4" t="s">
         <v>105</v>
       </c>
@@ -5614,14 +6039,14 @@
         <v>9.25</v>
       </c>
       <c r="I121" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>264.92</v>
       </c>
       <c r="J121" s="8">
         <v>215.97</v>
       </c>
       <c r="K121" s="9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>22.665184979395296</v>
       </c>
       <c r="M121" s="14">
@@ -5631,8 +6056,12 @@
         <v>4009</v>
       </c>
       <c r="O121" s="17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-10.871498443752779</v>
+      </c>
+      <c r="Q121" s="18" t="str">
+        <f t="shared" si="7"/>
+        <v>ici</v>
       </c>
     </row>
     <row r="134" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>